<commit_message>
edited Subscriber_Excel.py to add more graphs
</commit_message>
<xml_diff>
--- a/line.xlsx
+++ b/line.xlsx
@@ -249,11 +249,11 @@
         <axId val="500"/>
         <scaling>
           <orientation val="minMax"/>
-          <max val="7"/>
+          <max val="10"/>
           <min val="2"/>
         </scaling>
-        <delete val="0"/>
         <axPos val="l"/>
+        <minorGridlines/>
         <title>
           <tx>
             <rich>
@@ -270,7 +270,7 @@
           </tx>
         </title>
         <numFmt formatCode="dd/mm/yy-HH:MM" sourceLinked="0"/>
-        <majorTickMark val="none"/>
+        <majorTickMark val="cross"/>
         <minorTickMark val="none"/>
         <crossAx val="100"/>
         <majorTimeUnit val="days"/>
@@ -280,7 +280,6 @@
         <scaling>
           <orientation val="minMax"/>
         </scaling>
-        <delete val="0"/>
         <axPos val="l"/>
         <majorGridlines/>
         <title>
@@ -661,7 +660,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>10/03/2020-19:56:32</t>
+          <t>10/04/2020-19:09:58</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -677,7 +676,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>10/03/2020-19:56:33</t>
+          <t>10/04/2020-19:09:59</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -693,7 +692,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>10/03/2020-19:56:34</t>
+          <t>10/04/2020-19:10:00</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -709,7 +708,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>10/03/2020-19:56:35</t>
+          <t>10/04/2020-19:10:01</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -725,7 +724,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>10/03/2020-19:56:36</t>
+          <t>10/04/2020-19:10:02</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -741,7 +740,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>10/03/2020-19:56:37</t>
+          <t>10/04/2020-19:10:03</t>
         </is>
       </c>
       <c r="B7" t="n">

</xml_diff>